<commit_message>
WRI updates for RTMF
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\20201118 eps-india\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE4D269-1906-40C9-9438-66386A9FA2BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6813D052-8D89-4B5A-ACE0-5E051F3A0C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="2250" windowWidth="23595" windowHeight="14160" xr2:uid="{B1321729-65FD-4E39-A16A-F420F6CD402A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B1321729-65FD-4E39-A16A-F420F6CD402A}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -532,7 +531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A295D-ACEE-40E1-A0AB-57EEA1BFAA47}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -665,7 +666,9 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -848,13 +851,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -865,7 +868,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -889,7 +892,9 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -932,13 +937,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -949,7 +954,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="6">
         <f>1-SUM(B2:G2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -966,10 +971,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F3" s="4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -1072,13 +1077,13 @@
         <v>0</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -1089,7 +1094,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.33999999999999997</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
WRI edits for RTMF
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\20201118 eps-india\InputData\trans\RTMF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6813D052-8D89-4B5A-ACE0-5E051F3A0C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B1321729-65FD-4E39-A16A-F420F6CD402A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5730"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="RTMF-passengers" sheetId="2" r:id="rId2"/>
-    <sheet name="RTMF-freight" sheetId="3" r:id="rId3"/>
+    <sheet name="IndiaCalcs- Web Guidance" sheetId="4" r:id="rId2"/>
+    <sheet name="RTMF-passengers" sheetId="2" r:id="rId3"/>
+    <sheet name="RTMF-freight" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>RTMF Recipient Transportation Mode Fractions</t>
   </si>
@@ -142,11 +142,74 @@
   <si>
     <t>the following mode shifts:</t>
   </si>
+  <si>
+    <t>BAU</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>2ws</t>
+  </si>
+  <si>
+    <t>3ws</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>nmt</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>shift-to</t>
+  </si>
+  <si>
+    <t>shift-from</t>
+  </si>
+  <si>
+    <t>ratios of target modes</t>
+  </si>
+  <si>
+    <t>Sustainable Scenario</t>
+  </si>
+  <si>
+    <t>Mode shares in 2050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: </t>
+  </si>
+  <si>
+    <t>https://orbit.dtu.dk/files/120569095/Transport_Scenarios_for_India.pdf</t>
+  </si>
+  <si>
+    <t>Passenger Private Transport</t>
+  </si>
+  <si>
+    <t>Freight HDVs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"In the High Rail Scenario, a modal shift to </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rail occurs.. in freight transport (mainly) away </t>
+  </si>
+  <si>
+    <t>from heavy trucks"</t>
+  </si>
+  <si>
+    <t>https://www.iea.org/reports/the-future-of-rail</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -181,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,8 +257,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -203,11 +284,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -215,6 +324,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -230,6 +354,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>172463</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>182544</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AE3A85D-E566-4907-8CCC-8D20F9F02963}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7858125" y="0"/>
+          <a:ext cx="4954013" cy="2659044"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>548377</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>10094</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC61108-1913-413A-A894-2E04D3DC4B1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3057525" y="3400425"/>
+          <a:ext cx="5863327" cy="3658169"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,24 +745,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4A295D-ACEE-40E1-A0AB-57EEA1BFAA47}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -553,80 +770,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -635,7 +852,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -644,7 +861,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -660,24 +877,265 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5439016C-B89E-42B2-9367-3788A58F3CB4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.265625" customWidth="1"/>
+    <col min="6" max="6" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
+    <col min="10" max="10" width="20.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="E1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="9">
+        <v>25</v>
+      </c>
+      <c r="F3" s="9">
+        <v>19</v>
+      </c>
+      <c r="G3" s="13">
+        <f t="shared" ref="G3:G8" si="0">F3-E3</f>
+        <v>-6</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13">
+        <f>SUM(G3:G5)</f>
+        <v>-13</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="9">
+        <f>52-E3</f>
+        <v>27</v>
+      </c>
+      <c r="F4" s="9">
+        <f>40-F3</f>
+        <v>21</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="9">
+        <f>58-52</f>
+        <v>6</v>
+      </c>
+      <c r="F5" s="9">
+        <f>45-40</f>
+        <v>5</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="9">
+        <f>82-58</f>
+        <v>24</v>
+      </c>
+      <c r="F6" s="9">
+        <f>77-45</f>
+        <v>32</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H6" s="14">
+        <f>SUM(G6:G8)</f>
+        <v>13</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10">
+        <f>G6/$H$6</f>
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="9">
+        <f>91-82</f>
+        <v>9</v>
+      </c>
+      <c r="F7" s="9">
+        <f>88-77</f>
+        <v>11</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10">
+        <f>G7/$H$6</f>
+        <v>0.15384615384615385</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="9">
+        <f>100-91</f>
+        <v>9</v>
+      </c>
+      <c r="F8" s="9">
+        <f>100-88</f>
+        <v>12</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10">
+        <f>G8/$H$6</f>
+        <v>0.23076923076923078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E9" s="9">
+        <f>SUM(E3:E8)</f>
+        <v>100</v>
+      </c>
+      <c r="F9" s="9">
+        <f>SUM(F3:F8)</f>
+        <v>100</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="K16" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="8"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F39" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -703,21 +1161,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
-        <v>0.33</v>
+      <c r="C2" s="15">
+        <f>'IndiaCalcs- Web Guidance'!J6</f>
+        <v>0.61538461538461542</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
-      <c r="E2" s="4">
-        <v>0.33</v>
+      <c r="E2" s="15">
+        <f>'IndiaCalcs- Web Guidance'!J7</f>
+        <v>0.15384615384615385</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -726,12 +1186,12 @@
         <v>0</v>
       </c>
       <c r="H2" s="4"/>
-      <c r="I2" s="6">
+      <c r="I2" s="16">
         <f>1-SUM(B2:G2)</f>
-        <v>0.33999999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.23076923076923073</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -759,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -787,7 +1247,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -815,7 +1275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -843,21 +1303,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
       </c>
-      <c r="C7" s="4">
-        <v>0.33</v>
+      <c r="C7" s="15">
+        <f>C2</f>
+        <v>0.61538461538461542</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
-        <v>0.33</v>
+      <c r="E7" s="15">
+        <f>E2</f>
+        <v>0.15384615384615385</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -866,12 +1328,12 @@
         <v>0</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="I7" s="6">
+      <c r="I7" s="16">
         <f t="shared" si="0"/>
-        <v>0.33999999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.23076923076923073</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -885,25 +1347,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E2AAAC-5DEA-4554-803B-E8EE05A805DF}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.59765625" customWidth="1"/>
+    <col min="8" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -929,7 +1391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -957,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -971,10 +1433,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G3" s="4">
         <v>0</v>
@@ -985,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1041,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1097,7 +1559,7 @@
         <v>0.33999999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>

</xml_diff>